<commit_message>
Update PM20 Tidsregistrering for Patrick.xlsx
</commit_message>
<xml_diff>
--- a/08 Project Management/Tidsregistrering/PM20 Tidsregistrering for Patrick.xlsx
+++ b/08 Project Management/Tidsregistrering/PM20 Tidsregistrering for Patrick.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{226367E4-1D2F-4A4F-957F-7F07C108A4D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80B1473-7C2F-4966-8DAE-B5A46D5F2511}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
+    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8964" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Tidsregistrering af (Navn)</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>Gennemgang af GitHub Rep</t>
+  </si>
+  <si>
+    <t>Review på UC07</t>
+  </si>
+  <si>
+    <t>Merge på OC0803</t>
   </si>
 </sst>
 </file>
@@ -313,7 +319,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -358,13 +364,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent2" xfId="2" builtinId="33"/>
@@ -745,7 +754,7 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -760,16 +769,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
@@ -811,28 +820,42 @@
         <v>0.35416666666666669</v>
       </c>
       <c r="E3" s="14">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="F3" s="24">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F3" s="22">
         <v>0.10416666666666667</v>
       </c>
       <c r="G3" s="5">
         <f>E3-D3</f>
-        <v>0.10416666666666663</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H3" s="1">
         <f>SUM(G$3:G3)</f>
-        <v>0.10416666666666663</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="20"/>
+      <c r="A4" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="15">
+        <v>43893</v>
+      </c>
+      <c r="D4" s="16">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E4" s="16">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F4" s="25">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="G4" s="5">
         <f t="shared" ref="G4:G32" si="0">E4-D4</f>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="H4" s="1">
         <f>SUM(G$3:G4)</f>
@@ -840,17 +863,29 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
+      <c r="A5" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="15">
+        <v>43893</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E5" s="16">
+        <v>0.625</v>
+      </c>
       <c r="F5" s="20"/>
       <c r="G5" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="H5" s="1">
         <f>SUM(G$3:G5)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -864,7 +899,7 @@
       </c>
       <c r="H6" s="1">
         <f>SUM(G$3:G6)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -878,7 +913,7 @@
       </c>
       <c r="H7" s="1">
         <f>SUM(G$3:G7)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -892,7 +927,7 @@
       </c>
       <c r="H8" s="1">
         <f>SUM(G$3:G8)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -906,7 +941,7 @@
       </c>
       <c r="H9" s="1">
         <f>SUM(G$3:G9)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -920,7 +955,7 @@
       </c>
       <c r="H10" s="1">
         <f>SUM(G$3:G10)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -934,7 +969,7 @@
       </c>
       <c r="H11" s="1">
         <f>SUM(G$3:G11)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -948,7 +983,7 @@
       </c>
       <c r="H12" s="1">
         <f>SUM(G$3:G12)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -962,7 +997,7 @@
       </c>
       <c r="H13" s="1">
         <f>SUM(G$3:G13)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -974,7 +1009,7 @@
       </c>
       <c r="H14" s="1">
         <f>SUM(G$3:G14)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -986,7 +1021,7 @@
       </c>
       <c r="H15" s="1">
         <f>SUM(G$3:G15)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -998,7 +1033,7 @@
       </c>
       <c r="H16" s="1">
         <f>SUM(G$3:G16)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="17" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1010,7 +1045,7 @@
       </c>
       <c r="H17" s="1">
         <f>SUM(G$3:G17)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="18" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1022,7 +1057,7 @@
       </c>
       <c r="H18" s="1">
         <f>SUM(G$3:G18)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="19" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1034,7 +1069,7 @@
       </c>
       <c r="H19" s="1">
         <f>SUM(G$3:G19)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="20" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1046,7 +1081,7 @@
       </c>
       <c r="H20" s="1">
         <f>SUM(G$3:G20)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="21" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1058,7 +1093,7 @@
       </c>
       <c r="H21" s="1">
         <f>SUM(G$3:G21)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="22" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1070,7 +1105,7 @@
       </c>
       <c r="H22" s="1">
         <f>SUM(G$3:G22)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="23" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1082,7 +1117,7 @@
       </c>
       <c r="H23" s="1">
         <f>SUM(G$3:G23)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="24" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1094,7 +1129,7 @@
       </c>
       <c r="H24" s="1">
         <f>SUM(G$3:G24)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="25" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1105,7 +1140,7 @@
       </c>
       <c r="H25" s="1">
         <f>SUM(G$3:G25)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="26" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1116,7 +1151,7 @@
       </c>
       <c r="H26" s="1">
         <f>SUM(G$3:G26)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="27" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1127,7 +1162,7 @@
       </c>
       <c r="H27" s="1">
         <f>SUM(G$3:G27)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="28" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1138,7 +1173,7 @@
       </c>
       <c r="H28" s="1">
         <f>SUM(G$3:G28)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="29" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1149,7 +1184,7 @@
       </c>
       <c r="H29" s="1">
         <f>SUM(G$3:G29)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="30" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1160,7 +1195,7 @@
       </c>
       <c r="H30" s="1">
         <f>SUM(G$3:G30)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="31" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1171,7 +1206,7 @@
       </c>
       <c r="H31" s="1">
         <f>SUM(G$3:G31)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="32" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1182,7 +1217,7 @@
       </c>
       <c r="H32" s="1">
         <f>SUM(G$3:G32)</f>
-        <v>0.10416666666666663</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.3">
@@ -1267,13 +1302,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">

</xml_diff>